<commit_message>
Correct high-inertia local-mode simulation
</commit_message>
<xml_diff>
--- a/Examples/68Bus_HighInertia_LocalMode.xlsx
+++ b/Examples/68Bus_HighInertia_LocalMode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE50E8-65BD-4E92-AA4D-DADE7EC96334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D77974E-5142-42BD-BF5E-876D3AB3A90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3293,7 +3293,7 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3361,17 +3361,17 @@
         <v>0</v>
       </c>
       <c r="C4" s="9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D18" si="1">0.25*C4/10</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E4" s="9">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F4" s="9">
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="G4" s="7"/>
       <c r="J4" s="2"/>

</xml_diff>